<commit_message>
add all games to stats.xlsx
</commit_message>
<xml_diff>
--- a/statistics/HW1_stats.xlsx
+++ b/statistics/HW1_stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="201" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="171" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="58">
   <si>
     <t>Kattis score</t>
   </si>
@@ -44,6 +44,30 @@
     <t>PiecesLeader</t>
   </si>
   <si>
+    <t>vs</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>KingLeader</t>
+  </si>
+  <si>
+    <t>KingPenalty</t>
+  </si>
+  <si>
+    <t>Offense</t>
+  </si>
+  <si>
+    <t>DefenseSide</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>KingLeader + KingPenalty</t>
+  </si>
+  <si>
     <t>EndGame</t>
   </si>
   <si>
@@ -56,22 +80,43 @@
     <t>AB d=9 PL ( S15 )</t>
   </si>
   <si>
-    <t>KingLeader</t>
+    <t>( dd )</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>LW</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>DW</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>WD</t>
   </si>
   <si>
     <t>win</t>
   </si>
   <si>
-    <t>KingPenalty</t>
-  </si>
-  <si>
-    <t>Offense</t>
+    <t>D RTE</t>
+  </si>
+  <si>
+    <t>WL</t>
+  </si>
+  <si>
+    <t>DL</t>
   </si>
   <si>
     <t>AB d=9 PL+KP ( S17 )</t>
   </si>
   <si>
-    <t>DefenseSide</t>
+    <t>RTE D</t>
   </si>
   <si>
     <t>draw</t>
@@ -80,7 +125,7 @@
     <t>-</t>
   </si>
   <si>
-    <t>Defense</t>
+    <t>LL</t>
   </si>
   <si>
     <t>PiecesLeader + EndGame</t>
@@ -113,6 +158,18 @@
     <t>PiecesLeader + EndGame + KingPenalty</t>
   </si>
   <si>
+    <t>Win</t>
+  </si>
+  <si>
+    <t>Loose</t>
+  </si>
+  <si>
+    <t>Draw</t>
+  </si>
+  <si>
+    <t>Kattis Score</t>
+  </si>
+  <si>
     <t>PiecesLeader + EndGame + Offense</t>
   </si>
   <si>
@@ -122,10 +179,16 @@
     <t>PiecesLeader + EndGame + DefenseSide</t>
   </si>
   <si>
+    <t>Basic </t>
+  </si>
+  <si>
     <t>PiecesLeader + EndGame + Defense</t>
   </si>
   <si>
     <t>PiecesLeader + EndGame + KingPenalty + KingLeader</t>
+  </si>
+  <si>
+    <t>sum</t>
   </si>
 </sst>
 </file>
@@ -163,7 +226,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -180,13 +242,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
@@ -278,7 +340,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -303,15 +365,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,7 +389,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -340,6 +410,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,10 +438,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:K22"/>
+  <dimension ref="B3:T26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q27" activeCellId="0" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -376,7 +454,11 @@
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="44.015306122449"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.3061224489796"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.1122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.0051020408163"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="23.1275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -406,11 +488,21 @@
       <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="M4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
@@ -431,10 +523,34 @@
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8"/>
+      <c r="M5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>16</v>
@@ -448,19 +564,43 @@
       <c r="F6" s="4" t="n">
         <v>4.3</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>12</v>
+      <c r="N6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>13</v>
@@ -475,16 +615,40 @@
         <v>6.4</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="8" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>10</v>
@@ -501,10 +665,34 @@
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
       <c r="K8" s="8"/>
+      <c r="M8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>4</v>
@@ -518,19 +706,43 @@
       <c r="F9" s="4" t="n">
         <v>4.4</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>10</v>
+      <c r="I9" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>5</v>
@@ -545,18 +757,42 @@
         <v>4.2</v>
       </c>
       <c r="I10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>20</v>
+      <c r="N10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>1</v>
@@ -573,15 +809,39 @@
       <c r="I11" s="6"/>
       <c r="J11" s="7"/>
       <c r="K11" s="8"/>
+      <c r="M11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="11" t="s">
-        <v>22</v>
+      <c r="B12" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="D12" s="12" t="n">
+      <c r="D12" s="14" t="n">
         <v>18</v>
       </c>
       <c r="E12" s="4" t="n">
@@ -590,19 +850,43 @@
       <c r="F12" s="4" t="n">
         <v>5.4</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>10</v>
+      <c r="I12" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" s="9" t="s">
         <v>23</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>15</v>
@@ -617,16 +901,16 @@
         <v>5.5</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>17</v>
@@ -646,7 +930,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>12</v>
@@ -660,45 +944,45 @@
       <c r="F15" s="4" t="n">
         <v>8.3</v>
       </c>
-      <c r="I15" s="9" t="s">
-        <v>10</v>
+      <c r="I15" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>5</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>12.6</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>18</v>
@@ -717,8 +1001,8 @@
       <c r="K17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11" t="s">
-        <v>31</v>
+      <c r="B18" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>18</v>
@@ -732,45 +1016,73 @@
       <c r="F18" s="4" t="n">
         <v>5.8</v>
       </c>
-      <c r="I18" s="9" t="s">
-        <v>10</v>
+      <c r="I18" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="9"/>
+      <c r="N18" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D19" s="4" t="n">
         <v>18</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F19" s="4" t="n">
         <v>5.5</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="O19" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q19" s="9" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>18</v>
@@ -784,13 +1096,28 @@
       <c r="F20" s="4" t="n">
         <v>5.8</v>
       </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
+      <c r="M20" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="N20" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="O20" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="P20" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="9" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>17</v>
@@ -804,10 +1131,25 @@
       <c r="F21" s="4" t="n">
         <v>5.6</v>
       </c>
+      <c r="M21" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="O21" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="P21" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="12" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>18</v>
@@ -821,12 +1163,94 @@
       <c r="F22" s="4" t="n">
         <v>5.1</v>
       </c>
+      <c r="M22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="O22" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="P22" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="9" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="O23" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P23" s="9" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q23" s="9" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="P24" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="9" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M25" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O25" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="P25" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="9" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M26" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N26" s="19" t="n">
+        <f aca="false">N19+N20+N21+N22+N23+N24+N25</f>
+        <v>23</v>
+      </c>
+      <c r="O26" s="19" t="n">
+        <f aca="false">O25+O24+O23+O22+O21+O20+O19</f>
+        <v>23</v>
+      </c>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:K4"/>
+    <mergeCell ref="M4:T4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>